<commit_message>
Excel connected dependency is added
</commit_message>
<xml_diff>
--- a/seleniumSupport/ExcelFile/InputFormSubmitte.xlsx
+++ b/seleniumSupport/ExcelFile/InputFormSubmitte.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="15255" windowHeight="7950"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14475" windowHeight="6090"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="100">
   <si>
     <t>LastName</t>
   </si>
@@ -685,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1053,6 +1054,11 @@
       </c>
       <c r="J11" s="1" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>